<commit_message>
Create Statements angepasst. Testdatensätze für alle Filter erstellt. Systemspezifikation für die Filtertypen angepasst. Aussehen der erweiterten Suche weiter angepasst.
</commit_message>
<xml_diff>
--- a/docs/Systemspezifikation/Filtertypen.xlsx
+++ b/docs/Systemspezifikation/Filtertypen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahri\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3106F7D2-26A7-4E0D-A8E8-07118E1CE648}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4B7AAB-2397-47A9-96CB-EC71A3FEA977}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" xr2:uid="{0DAD7B02-AF67-4603-B4AE-30319D9428BC}"/>
   </bookViews>
@@ -205,6 +205,21 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -279,21 +294,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -308,15 +308,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBBF1ADA-1769-4FDD-AC43-3BC1BBA131FF}" name="Tabelle1" displayName="Tabelle1" ref="B1:D37" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBBF1ADA-1769-4FDD-AC43-3BC1BBA131FF}" name="Tabelle1" displayName="Tabelle1" ref="B1:D37" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="B1:D37" xr:uid="{138BDC3A-0BED-433B-A0D2-83DAC75FAA6B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B37">
     <sortCondition ref="B1:B37"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{033E41F1-C7EA-4E94-8B13-CD1D04D7D81E}" name="Filtername" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{DF21FE13-A77B-4569-8455-543140646B49}" name="Typ" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{BC58B583-3236-46EB-A71B-5A080FB06BF9}" name="Nummer" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{033E41F1-C7EA-4E94-8B13-CD1D04D7D81E}" name="Filtername" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{DF21FE13-A77B-4569-8455-543140646B49}" name="Typ" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{BC58B583-3236-46EB-A71B-5A080FB06BF9}" name="Nummer" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -632,7 +632,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,7 +791,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -1163,30 +1163,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C37">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Integer">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Integer">
       <formula>NOT(ISERROR(SEARCH("Integer",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Schieberegler">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Schieberegler">
       <formula>NOT(ISERROR(SEARCH("Schieberegler",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Dropdown">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Dropdown">
       <formula>NOT(ISERROR(SEARCH("Dropdown",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Checkbox">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Checkbox">
       <formula>NOT(ISERROR(SEARCH("Checkbox",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D37">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>